<commit_message>
adding a bigger table
</commit_message>
<xml_diff>
--- a/data-raw/Performance_sportive_et_nb_points.xlsx
+++ b/data-raw/Performance_sportive_et_nb_points.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="79">
   <si>
     <t>Fonction</t>
   </si>
@@ -82,6 +82,180 @@
   </si>
   <si>
     <t>Grenadier - Isone, Char or Military Police</t>
+  </si>
+  <si>
+    <t>Motorist for special vehicles</t>
+  </si>
+  <si>
+    <t>Dog handler</t>
+  </si>
+  <si>
+    <t>Artillery driver</t>
+  </si>
+  <si>
+    <t>Construction machinery Operator</t>
+  </si>
+  <si>
+    <t>Driver of NBC detection vehicles</t>
+  </si>
+  <si>
+    <t>NBC exploration vehicle Driver</t>
+  </si>
+  <si>
+    <t>Artillery Tracked Vehicle Driver</t>
+  </si>
+  <si>
+    <t>Cook (Civil Protection)</t>
+  </si>
+  <si>
+    <t>Diagnostician of the Swiss Control Network</t>
+  </si>
+  <si>
+    <t>Radio Explorer</t>
+  </si>
+  <si>
+    <t>Strategic radio Explorer (Long Service)</t>
+  </si>
+  <si>
+    <t>Parachute Scout</t>
+  </si>
+  <si>
+    <t>Crew Infantryman</t>
+  </si>
+  <si>
+    <t>Blacksmith</t>
+  </si>
+  <si>
+    <t>Officers' orders</t>
+  </si>
+  <si>
+    <t>Drone Pilot / Operator</t>
+  </si>
+  <si>
+    <t>Pioneer (Civil Protection)</t>
+  </si>
+  <si>
+    <t>Pioneer of directed wave technology</t>
+  </si>
+  <si>
+    <t>Bridge Operator</t>
+  </si>
+  <si>
+    <t>Bridge Operator / Bellman</t>
+  </si>
+  <si>
+    <t>Materielman (Civil Protection)</t>
+  </si>
+  <si>
+    <t>Assistance Officer (Civil Protection)</t>
+  </si>
+  <si>
+    <t>Driver's aid Attendant (Civil Protection)</t>
+  </si>
+  <si>
+    <t>Infrastructure Officer (Civil Protection)</t>
+  </si>
+  <si>
+    <t>Rescue Equipment Operator</t>
+  </si>
+  <si>
+    <t>Unit Sanitarian / Sanitary Tank Driver</t>
+  </si>
+  <si>
+    <t>Unit Sanitary - Driver C1</t>
+  </si>
+  <si>
+    <t>Sapper</t>
+  </si>
+  <si>
+    <t>Tank Sapper</t>
+  </si>
+  <si>
+    <t>Secretary</t>
+  </si>
+  <si>
+    <t>Cyber Soldier</t>
+  </si>
+  <si>
+    <t>Hospital Soldier</t>
+  </si>
+  <si>
+    <t>Grenadier Tank Crew Soldier</t>
+  </si>
+  <si>
+    <t>Tank Soldier</t>
+  </si>
+  <si>
+    <t>Tank Support Trooper</t>
+  </si>
+  <si>
+    <t>Fire Marshal</t>
+  </si>
+  <si>
+    <t>NBC Defense Soldier Decontamination</t>
+  </si>
+  <si>
+    <t>NBC Defense Soldier Detection</t>
+  </si>
+  <si>
+    <t>Traffic Soldier</t>
+  </si>
+  <si>
+    <t>Logistics Soldier</t>
+  </si>
+  <si>
+    <t>Kitchen Logistics Soldier</t>
+  </si>
+  <si>
+    <t>Soldier in the Military Band</t>
+  </si>
+  <si>
+    <t>Military Police Soldier</t>
+  </si>
+  <si>
+    <t>Driving Echelon Soldier</t>
+  </si>
+  <si>
+    <t>Radar Soldier</t>
+  </si>
+  <si>
+    <t>Air Force Intelligence Soldier</t>
+  </si>
+  <si>
+    <t>Rescue Trooper</t>
+  </si>
+  <si>
+    <t>Sports Soldier</t>
+  </si>
+  <si>
+    <t>Safety Soldier</t>
+  </si>
+  <si>
+    <t>Telematics Soldier</t>
+  </si>
+  <si>
+    <t>Telematics Soldier / Language Specialist Candidate</t>
+  </si>
+  <si>
+    <t>Train Soldier</t>
+  </si>
+  <si>
+    <t>STINGER Guided Machine Soldier</t>
+  </si>
+  <si>
+    <t>Operations Soldier (training and support)</t>
+  </si>
+  <si>
+    <t>Technical Hospital Soldier</t>
+  </si>
+  <si>
+    <t>Construction Soldier</t>
+  </si>
+  <si>
+    <t>Health Soldier - Medical Region</t>
+  </si>
+  <si>
+    <t>Veterinarian Soldier</t>
   </si>
 </sst>
 </file>
@@ -162,7 +336,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -171,6 +345,12 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -444,7 +624,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -452,10 +632,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B78"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A20"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="C79" sqref="C79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -625,6 +805,470 @@
         <v>90</v>
       </c>
     </row>
+    <row r="21" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="7">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="7">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="7">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" s="7">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" s="7">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="7">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" s="7">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29" s="7">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30" s="7">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31" s="7">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B32" s="7">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B33" s="7">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B34" s="7">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B35" s="7">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B36" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B37" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B38" s="7">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B39" s="7">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B40" s="7">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B41" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B42" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B43" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B44" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B45" s="7">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B46" s="7">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B47" s="7">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B48" s="7">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B49" s="7">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B50" s="7">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B51" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B52" s="7">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B53" s="7">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B54" s="7">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B55" s="7">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B56" s="7">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A57" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B57" s="7">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A58" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B58" s="7">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B59" s="7">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A60" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B60" s="7">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A61" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B61" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A62" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B62" s="7">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A63" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B63" s="7">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A64" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B64" s="7">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A65" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B65" s="7">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A66" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B66" s="7">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A67" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B67" s="7">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A68" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B68" s="7">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A69" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B69" s="7">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A70" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B70" s="7">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A71" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B71" s="7">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A72" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B72" s="7">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A73" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B73" s="7">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A74" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B74" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A75" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B75" s="7">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A76" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B76" s="7">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A77" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B77" s="7">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A78" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B78" s="7">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:D21">
     <sortCondition ref="B2:B21"/>

</xml_diff>

<commit_message>
Update of the shiny app directely into the package
</commit_message>
<xml_diff>
--- a/data-raw/Performance_sportive_et_nb_points.xlsx
+++ b/data-raw/Performance_sportive_et_nb_points.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="85">
   <si>
     <t>Fonction</t>
   </si>
@@ -27,245 +27,271 @@
     <t>min nb points</t>
   </si>
   <si>
-    <t>Fusilier</t>
-  </si>
-  <si>
-    <t>Pilot</t>
-  </si>
-  <si>
-    <t>Company Accountant</t>
-  </si>
-  <si>
-    <t>Troop Cook</t>
-  </si>
-  <si>
-    <t>Office Order</t>
-  </si>
-  <si>
-    <t>Cannoneer</t>
-  </si>
-  <si>
-    <t>Mechanic</t>
-  </si>
-  <si>
-    <t>Intelligence Soldier</t>
-  </si>
-  <si>
-    <t>Transmission Soldier</t>
-  </si>
-  <si>
-    <t>Driver</t>
-  </si>
-  <si>
-    <t>Cannonballer</t>
-  </si>
-  <si>
-    <t>Infantryman</t>
-  </si>
-  <si>
-    <t>Sanitary</t>
-  </si>
-  <si>
-    <t>Artillery Soldier</t>
-  </si>
-  <si>
-    <t>Air Force Soldier</t>
-  </si>
-  <si>
-    <t>Explorer</t>
-  </si>
-  <si>
-    <t>Scout</t>
-  </si>
-  <si>
-    <t>Mountain Specialist</t>
-  </si>
-  <si>
-    <t>Grenadier - Isone, Char or Military Police</t>
-  </si>
-  <si>
-    <t>Motorist for special vehicles</t>
-  </si>
-  <si>
-    <t>Dog handler</t>
-  </si>
-  <si>
-    <t>Artillery driver</t>
-  </si>
-  <si>
-    <t>Construction machinery Operator</t>
-  </si>
-  <si>
-    <t>Driver of NBC detection vehicles</t>
-  </si>
-  <si>
-    <t>NBC exploration vehicle Driver</t>
-  </si>
-  <si>
-    <t>Artillery Tracked Vehicle Driver</t>
-  </si>
-  <si>
-    <t>Cook (Civil Protection)</t>
-  </si>
-  <si>
-    <t>Diagnostician of the Swiss Control Network</t>
-  </si>
-  <si>
-    <t>Radio Explorer</t>
-  </si>
-  <si>
-    <t>Strategic radio Explorer (Long Service)</t>
-  </si>
-  <si>
-    <t>Parachute Scout</t>
-  </si>
-  <si>
-    <t>Crew Infantryman</t>
-  </si>
-  <si>
-    <t>Blacksmith</t>
-  </si>
-  <si>
-    <t>Officers' orders</t>
-  </si>
-  <si>
-    <t>Drone Pilot / Operator</t>
-  </si>
-  <si>
-    <t>Pioneer (Civil Protection)</t>
-  </si>
-  <si>
-    <t>Pioneer of directed wave technology</t>
-  </si>
-  <si>
-    <t>Bridge Operator</t>
-  </si>
-  <si>
-    <t>Bridge Operator / Bellman</t>
-  </si>
-  <si>
-    <t>Materielman (Civil Protection)</t>
-  </si>
-  <si>
-    <t>Assistance Officer (Civil Protection)</t>
-  </si>
-  <si>
-    <t>Driver's aid Attendant (Civil Protection)</t>
-  </si>
-  <si>
-    <t>Infrastructure Officer (Civil Protection)</t>
-  </si>
-  <si>
-    <t>Rescue Equipment Operator</t>
-  </si>
-  <si>
-    <t>Unit Sanitarian / Sanitary Tank Driver</t>
-  </si>
-  <si>
-    <t>Unit Sanitary - Driver C1</t>
-  </si>
-  <si>
-    <t>Sapper</t>
-  </si>
-  <si>
-    <t>Tank Sapper</t>
-  </si>
-  <si>
-    <t>Secretary</t>
-  </si>
-  <si>
-    <t>Cyber Soldier</t>
-  </si>
-  <si>
-    <t>Hospital Soldier</t>
-  </si>
-  <si>
-    <t>Grenadier Tank Crew Soldier</t>
-  </si>
-  <si>
-    <t>Tank Soldier</t>
-  </si>
-  <si>
-    <t>Tank Support Trooper</t>
-  </si>
-  <si>
-    <t>Fire Marshal</t>
-  </si>
-  <si>
-    <t>NBC Defense Soldier Decontamination</t>
-  </si>
-  <si>
-    <t>NBC Defense Soldier Detection</t>
-  </si>
-  <si>
-    <t>Traffic Soldier</t>
-  </si>
-  <si>
-    <t>Logistics Soldier</t>
-  </si>
-  <si>
-    <t>Kitchen Logistics Soldier</t>
-  </si>
-  <si>
-    <t>Soldier in the Military Band</t>
-  </si>
-  <si>
-    <t>Military Police Soldier</t>
-  </si>
-  <si>
-    <t>Driving Echelon Soldier</t>
-  </si>
-  <si>
-    <t>Radar Soldier</t>
-  </si>
-  <si>
-    <t>Air Force Intelligence Soldier</t>
-  </si>
-  <si>
-    <t>Rescue Trooper</t>
-  </si>
-  <si>
-    <t>Sports Soldier</t>
-  </si>
-  <si>
-    <t>Safety Soldier</t>
-  </si>
-  <si>
-    <t>Telematics Soldier</t>
-  </si>
-  <si>
-    <t>Telematics Soldier / Language Specialist Candidate</t>
-  </si>
-  <si>
-    <t>Train Soldier</t>
-  </si>
-  <si>
-    <t>STINGER Guided Machine Soldier</t>
-  </si>
-  <si>
-    <t>Operations Soldier (training and support)</t>
-  </si>
-  <si>
-    <t>Technical Hospital Soldier</t>
-  </si>
-  <si>
-    <t>Construction Soldier</t>
-  </si>
-  <si>
-    <t>Health Soldier - Medical Region</t>
-  </si>
-  <si>
-    <t>Veterinarian Soldier</t>
+    <t>&lt;a href="https://www.miljobs.ch/fr/functions/comptable-de-troupe"&gt;Company Accountant&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.miljobs.ch/fr/functions/cuisinier-de-troupe"&gt;Troop Cook&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.miljobs.ch/fr/functions/ordonnance-de-bureau"&gt;Office Order&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.miljobs.ch/fr/functions/cuisinier-protection-civile"&gt;Cook (Civil Protection)&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.miljobs.ch/fr/functions/pilote-de-drones-operateur-de-charges-utiles-de-drones"&gt;Drone Pilot / Operator&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.miljobs.ch/fr/functions/pionnier-protection-civile"&gt;Pioneer (Civil Protection)&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.miljobs.ch/fr/functions/prepose-au-materiel-protection-civile"&gt;Materielman (Civil Protection)&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.miljobs.ch/fr/functions/prepose-a-lassistance-protection-civile"&gt;Assistance Officer (Civil Protection)&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.miljobs.ch/fr/functions/prepose-a-laide-a-la-conduite-protection-civile"&gt;Driver's aid Attendant (Civil Protection)&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.miljobs.ch/fr/functions/prepose-a-linfrastructure-protection-civile"&gt;Infrastructure Officer (Civil Protection)&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.miljobs.ch/fr/functions/soldat-cyber"&gt;Cyber Soldier&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.miljobs.ch/fr/functions/soldat-de-la-logistique-de-cuisine"&gt;Kitchen Logistics Soldier&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.miljobs.ch/fr/functions/soldat-dexploitation-instruction-et-support"&gt;Operations Soldier (training and support)&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.miljobs.ch/fr/functions/canonnier"&gt;Cannoneer&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.miljobs.ch/fr/functions/fusilier-de-bord"&gt;Fusilier&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.miljobs.ch/fr/functions/mecanicien-sur-appareils"&gt;Mechanic on equipment &lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.miljobs.ch/fr/functions/mecanicien-sur-appareils-de-renseignement-des-forces-aeriennes"&gt;mechanic on air force intelligence aircraft&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.miljobs.ch/fr/functions/mecanicien-sur-armes"&gt;weapons mechanic&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.miljobs.ch/fr/functions/mecanicien-sur-chars"&gt;mechanic on tanks&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.miljobs.ch/fr/functions/mecanicien-sur-moteurs"&gt;mechanic on engines&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.miljobs.ch/fr/functions/soldat-de-renseignement"&gt;Intelligence Soldier&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.miljobs.ch/fr/functions/soldat-des-transmissions"&gt;Transmission Soldier&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.miljobs.ch/fr/functions/conducteur-de-lartillerie"&gt;Artillery driver&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.miljobs.ch/fr/functions/conducteur-de-machines-de-chantier"&gt;Construction machinery Operator&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.miljobs.ch/fr/functions/conducteur-de-vehicules-de-detection-nbc"&gt;Driver of NBC detection vehicles&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.miljobs.ch/fr/functions/conducteur-de-vehicules-dexploration-nbc"&gt;NBC exploration vehicle Driver&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.miljobs.ch/fr/functions/diagnosticien-reseau-de-conduite-suisse"&gt;Diagnostician of the Swiss Control Network&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.miljobs.ch/fr/functions/explorateur-radio"&gt;Radio Explorer&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.miljobs.ch/fr/functions/explorateur-radio-strategique"&gt;Strategic radio Explorer (Long Service)&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.miljobs.ch/fr/functions/marechal-ferrant"&gt;Blacksmith&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.miljobs.ch/fr/functions/ordonnance-dofficiers"&gt;Officers' orders&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.miljobs.ch/fr/functions/pionnier-dondes-dirigees"&gt;Pioneer of directed wave technology&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.miljobs.ch/fr/functions/pontonnier"&gt;Bridge Operator&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.miljobs.ch/fr/functions/pontonnier-de-sonnettes"&gt;Bridge Operator / Bellman&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.miljobs.ch/fr/functions/prepose-aux-engins-de-sauvetage"&gt;Rescue Equipment Operator&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.miljobs.ch/fr/functions/secretaire"&gt;Secretary&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.miljobs.ch/fr/functions/soldat-dhopital"&gt;Hospital Soldier&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.miljobs.ch/fr/functions/soldat-de-direction-des-feux"&gt;Fire Marshal&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.miljobs.ch/fr/functions/soldat-de-defense-nbc-decontamination"&gt;NBC Defense Soldier Decontamination&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.miljobs.ch/fr/functions/soldat-de-defense-nbc-detection"&gt;NBC Defense Soldier Detection&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.miljobs.ch/fr/functions/soldat-de-la-logistique"&gt;Logistics Soldier&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.miljobs.ch/fr/functions/soldat-de-la-musique-militaire"&gt;Soldier in the Military Band&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.miljobs.ch/fr/functions/soldat-de-lechelon-de-conduite"&gt;Driving Echelon Soldier&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.miljobs.ch/fr/functions/soldat-de-radar"&gt;Radar Soldier&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.miljobs.ch/fr/functions/soldat-de-renseignement-des-forces-aeriennes"&gt;Air Force Intelligence Soldier&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.miljobs.ch/fr/functions/soldat-de-telematique"&gt;Telematics Soldier&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.miljobs.ch/fr/functions/soldat-de-telematique-candidat-specialiste-de-langues"&gt;Telematics Soldier / Language Specialist Candidate&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.miljobs.ch/fr/functions/soldat-dengins-guides-stinger"&gt;STINGER Guided Machine Soldier&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.miljobs.ch/fr/functions/soldat-dhopital-technique"&gt;Technical Hospital Soldier&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.miljobs.ch/fr/functions/soldat-douvrage"&gt;Construction Soldier&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.miljobs.ch/fr/functions/soldat-sanitaire-region-medico-militaire"&gt;Health Soldier - Medical Region&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.miljobs.ch/fr/functions/soldat-veterinaire"&gt;Veterinarian Soldier&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.miljobs.ch/fr/functions/automobiliste"&gt;Driver&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.miljobs.ch/fr/functions/automobiliste-vehicules-speciaux"&gt;Motorist for special vehicles&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.miljobs.ch/fr/functions/conducteur-de-chiens"&gt;Dog handler&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.miljobs.ch/fr/functions/soldat-de-la-circulation"&gt;Traffic Soldier&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.miljobs.ch/fr/functions/canonnier-lance-mines"&gt;Cannonballer&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.miljobs.ch/fr/functions/fantassin"&gt;Infantryman&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.miljobs.ch/fr/functions/soldat-sanitaire"&gt;Sanitary&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.miljobs.ch/fr/functions/soldat-dartillerie"&gt;Artillery Soldier&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.miljobs.ch/fr/functions/soldat-daviation-soldat-daerodrome"&gt;Air Force Soldier&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.miljobs.ch/fr/functions/conducteur-de-vehicules-a-chenilles-de-lartillerie"&gt;Artillery Tracked Vehicle Driver&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.miljobs.ch/fr/functions/fantassin-dequipage"&gt;Crew Infantryman&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.miljobs.ch/fr/functions/sanitaire-dunite"&gt;Unit Sanitarian / Sanitary Tank Driver&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.miljobs.ch/fr/functions/sanitaire-dunite-conducteur-c1"&gt;Unit Sanitary - Driver C1&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.miljobs.ch/fr/functions/sapeur"&gt;Sapper&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.miljobs.ch/fr/functions/soldat-dequipage-de-chars"&gt;Grenadier Tank Crew Soldier&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.miljobs.ch/fr/functions/soldat-de-chars"&gt;Tank Soldier&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.miljobs.ch/fr/functions/soldat-de-chars-dappui"&gt;Tank Support Trooper&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.miljobs.ch/fr/functions/soldat-de-sauvetage"&gt;Rescue Trooper&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.miljobs.ch/fr/functions/soldat-de-surete"&gt;Safety Soldier&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.miljobs.ch/fr/functions/soldat-du-train"&gt;Train Soldier&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.miljobs.ch/fr/functions/soldat-de-la-police-militaire"&gt;Military Police Soldier&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.miljobs.ch/fr/functions/pilote-militaire-fonction-professionnelle"&gt;Pilot&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.miljobs.ch/fr/functions/eclaireur-parachutiste"&gt;Parachute Scout&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.miljobs.ch/fr/functions/sapeur-de-chars"&gt;Tank Sapper&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.miljobs.ch/fr/functions/soldat-sport"&gt;Sports Soldier&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.miljobs.ch/fr/functions/explorateur"&gt;Explorer&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.miljobs.ch/fr/functions/eclaireur"&gt;Scout&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.miljobs.ch/fr/functions/specialiste-de-montagne"&gt;Mountain Specialist&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.miljobs.ch/fr/functions/grenadier"&gt;Grenadier - Isone&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.miljobs.ch/fr/functions/grenadier-de-chars"&gt;Tank grenadier&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.miljobs.ch/fr/functions/grenadier-de-la-police-militaire"&gt;military police grenadier&lt;/a&gt;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -333,16 +359,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
@@ -359,8 +383,12 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -639,10 +667,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1000"/>
+  <dimension ref="A1:B1004"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C78" sqref="C78"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -660,645 +688,669 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:2" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B4" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
+    <row r="5" spans="1:2" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B5" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
+    <row r="6" spans="1:2" ht="87" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B6" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
+    <row r="7" spans="1:2" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="87" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="87" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="87" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="87" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="87" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" s="3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="87" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" s="3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="87" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="87" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" s="3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="87" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
+      <c r="B28" s="3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29" s="3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30" s="3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31" s="3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B32" s="3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B33" s="3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B34" s="3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B35" s="3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
+      <c r="B36" s="3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
+      <c r="B37" s="3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B38" s="3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B39" s="3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="87" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B40" s="3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B8" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
+      <c r="B41" s="3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B9" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
+      <c r="B42" s="3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
+      <c r="B43" s="3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B11" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
+      <c r="B44" s="3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B45" s="3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="87" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B46" s="3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B47" s="3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="115.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B48" s="3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B49" s="3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B50" s="3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="B12" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="1" t="s">
+      <c r="B51" s="3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="87" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B52" s="3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B53" s="3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B54" s="4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B55" s="4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B56" s="4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A57" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B57" s="4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A58" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B58" s="4">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B59" s="4">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A60" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B60" s="4">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A61" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="B13" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="1" t="s">
+      <c r="B61" s="4">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A62" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B62" s="4">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="87" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A63" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B63" s="4">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A64" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B64" s="4">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A65" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B65" s="4">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A66" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B66" s="4">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A67" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B67" s="4">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A68" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B68" s="4">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A69" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B69" s="4">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A70" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B70" s="4">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A71" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B71" s="4">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A72" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B72" s="4">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A73" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B73" s="4">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A74" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="B14" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15" s="4">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B16" s="4">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B17" s="4">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B18" s="4">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B19" s="4">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B20" s="4">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B21" s="4">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B22" s="4">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B23" s="4">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B24" s="4">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B25" s="4">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B26" s="4">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B27" s="4">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B28" s="4">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B29" s="4">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B30" s="4">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B31" s="4">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B32" s="4">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B33" s="4">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B34" s="4">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B35" s="4">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B36" s="4">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B37" s="4">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B38" s="4">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B39" s="4">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B40" s="4">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B41" s="4">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B42" s="4">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="1" t="s">
+      <c r="B74" s="5">
         <v>70</v>
       </c>
-      <c r="B43" s="4">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B44" s="4">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B45" s="4">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="1" t="s">
+    </row>
+    <row r="75" spans="1:2" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A75" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="B46" s="4">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="1" t="s">
+      <c r="B75" s="5">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A76" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="B47" s="4">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="1" t="s">
+      <c r="B76" s="5">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A77" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="B48" s="4">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="1" t="s">
+      <c r="B77" s="5">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A78" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="B49" s="4">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B50" s="5">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B51" s="5">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B52" s="5">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B53" s="5">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B54" s="5">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B55" s="5">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B56" s="5">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B57" s="5">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B58" s="5">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B59" s="5">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B60" s="5">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B61" s="5">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A62" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B62" s="5">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A63" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B63" s="5">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B64" s="5">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A65" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B65" s="5">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A66" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B66" s="5">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A67" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B67" s="5">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A68" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B68" s="5">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A69" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B69" s="5">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A70" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B70" s="6">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A71" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B71" s="6">
+      <c r="B78" s="5">
         <v>80</v>
       </c>
     </row>
-    <row r="72" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A72" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B72" s="6">
+    <row r="79" spans="1:2" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A79" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="B79" s="5">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A80" s="7" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="73" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A73" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B73" s="6">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A74" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B74" s="6">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A75" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B75" s="6">
+      <c r="B80" s="5">
         <v>85</v>
       </c>
     </row>
-    <row r="76" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A76" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B76" s="6">
+    <row r="81" spans="1:2" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A81" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B81" s="5">
         <v>85</v>
       </c>
     </row>
-    <row r="77" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A77" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B77" s="6">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A78" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B78" s="7">
+    <row r="82" spans="1:2" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A82" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B82" s="6">
         <v>90</v>
       </c>
     </row>
-    <row r="79" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A79" s="1"/>
-      <c r="B79" s="1"/>
-    </row>
-    <row r="80" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A80" s="1"/>
-      <c r="B80" s="1"/>
-    </row>
-    <row r="81" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A81" s="1"/>
-      <c r="B81" s="1"/>
-    </row>
-    <row r="82" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A82" s="1"/>
-      <c r="B82" s="1"/>
-    </row>
-    <row r="83" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A83" s="1"/>
-      <c r="B83" s="1"/>
-    </row>
-    <row r="84" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A84" s="1"/>
-      <c r="B84" s="1"/>
+    <row r="83" spans="1:2" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A83" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="B83" s="6">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A84" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B84" s="6">
+        <v>90</v>
+      </c>
     </row>
     <row r="85" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A85" s="1"/>
@@ -4963,12 +5015,108 @@
     <row r="1000" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1000" s="1"/>
       <c r="B1000" s="1"/>
+    </row>
+    <row r="1001" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1001" s="1"/>
+      <c r="B1001" s="1"/>
+    </row>
+    <row r="1002" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1002" s="1"/>
+      <c r="B1002" s="1"/>
+    </row>
+    <row r="1003" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1003" s="1"/>
+      <c r="B1003" s="1"/>
+    </row>
+    <row r="1004" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1004" s="1"/>
+      <c r="B1004" s="1"/>
     </row>
   </sheetData>
   <sortState ref="A2:D21">
     <sortCondition ref="B2:B21"/>
   </sortState>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="https://www.miljobs.ch/fr/functions/comptable-de-troupe"/>
+    <hyperlink ref="A3" r:id="rId2" display="https://www.miljobs.ch/fr/functions/cuisinier-de-troupe"/>
+    <hyperlink ref="A4" r:id="rId3" display="https://www.miljobs.ch/fr/functions/ordonnance-de-bureau"/>
+    <hyperlink ref="A5" r:id="rId4" display="https://www.miljobs.ch/fr/functions/cuisinier-protection-civile"/>
+    <hyperlink ref="A6" r:id="rId5" display="https://www.miljobs.ch/fr/functions/pilote-de-drones-operateur-de-charges-utiles-de-drones"/>
+    <hyperlink ref="A7" r:id="rId6" display="https://www.miljobs.ch/fr/functions/pionnier-protection-civile"/>
+    <hyperlink ref="A8" r:id="rId7" display="https://www.miljobs.ch/fr/functions/prepose-au-materiel-protection-civile"/>
+    <hyperlink ref="A9" r:id="rId8" display="https://www.miljobs.ch/fr/functions/prepose-a-lassistance-protection-civile"/>
+    <hyperlink ref="A10" r:id="rId9" display="https://www.miljobs.ch/fr/functions/prepose-a-laide-a-la-conduite-protection-civile"/>
+    <hyperlink ref="A11" r:id="rId10" display="https://www.miljobs.ch/fr/functions/prepose-a-linfrastructure-protection-civile"/>
+    <hyperlink ref="A12" r:id="rId11" display="https://www.miljobs.ch/fr/functions/soldat-cyber"/>
+    <hyperlink ref="A13" r:id="rId12" display="https://www.miljobs.ch/fr/functions/soldat-de-la-logistique-de-cuisine"/>
+    <hyperlink ref="A14" r:id="rId13" display="https://www.miljobs.ch/fr/functions/soldat-dexploitation-instruction-et-support"/>
+    <hyperlink ref="A15" r:id="rId14" display="https://www.miljobs.ch/fr/functions/canonnier"/>
+    <hyperlink ref="A16" r:id="rId15" display="https://www.miljobs.ch/fr/functions/fusilier-de-bord"/>
+    <hyperlink ref="A22" r:id="rId16" display="https://www.miljobs.ch/fr/functions/soldat-de-renseignement"/>
+    <hyperlink ref="A23" r:id="rId17" display="https://www.miljobs.ch/fr/functions/soldat-des-transmissions"/>
+    <hyperlink ref="A24" r:id="rId18" display="https://www.miljobs.ch/fr/functions/conducteur-de-lartillerie"/>
+    <hyperlink ref="A25" r:id="rId19" display="https://www.miljobs.ch/fr/functions/conducteur-de-machines-de-chantier"/>
+    <hyperlink ref="A26" r:id="rId20" display="https://www.miljobs.ch/fr/functions/conducteur-de-vehicules-de-detection-nbc"/>
+    <hyperlink ref="A27" r:id="rId21" display="https://www.miljobs.ch/fr/functions/conducteur-de-vehicules-dexploration-nbc"/>
+    <hyperlink ref="A28" r:id="rId22" display="https://www.miljobs.ch/fr/functions/diagnosticien-reseau-de-conduite-suisse"/>
+    <hyperlink ref="A29" r:id="rId23" display="https://www.miljobs.ch/fr/functions/explorateur-radio"/>
+    <hyperlink ref="A30" r:id="rId24" display="https://www.miljobs.ch/fr/functions/explorateur-radio-strategique"/>
+    <hyperlink ref="A31" r:id="rId25" display="https://www.miljobs.ch/fr/functions/marechal-ferrant"/>
+    <hyperlink ref="A32" r:id="rId26" display="https://www.miljobs.ch/fr/functions/ordonnance-dofficiers"/>
+    <hyperlink ref="A33" r:id="rId27" display="https://www.miljobs.ch/fr/functions/pionnier-dondes-dirigees"/>
+    <hyperlink ref="A34" r:id="rId28" display="https://www.miljobs.ch/fr/functions/pontonnier"/>
+    <hyperlink ref="A35" r:id="rId29" display="https://www.miljobs.ch/fr/functions/pontonnier-de-sonnettes"/>
+    <hyperlink ref="A36" r:id="rId30" display="https://www.miljobs.ch/fr/functions/prepose-aux-engins-de-sauvetage"/>
+    <hyperlink ref="A37" r:id="rId31" display="https://www.miljobs.ch/fr/functions/secretaire"/>
+    <hyperlink ref="A38" r:id="rId32" display="https://www.miljobs.ch/fr/functions/soldat-dhopital"/>
+    <hyperlink ref="A39" r:id="rId33" display="https://www.miljobs.ch/fr/functions/soldat-de-direction-des-feux"/>
+    <hyperlink ref="A40" r:id="rId34" display="https://www.miljobs.ch/fr/functions/soldat-de-defense-nbc-decontamination"/>
+    <hyperlink ref="A41" r:id="rId35" display="https://www.miljobs.ch/fr/functions/soldat-de-defense-nbc-detection"/>
+    <hyperlink ref="A42" r:id="rId36" display="https://www.miljobs.ch/fr/functions/soldat-de-la-logistique"/>
+    <hyperlink ref="A43" r:id="rId37" display="https://www.miljobs.ch/fr/functions/soldat-de-la-musique-militaire"/>
+    <hyperlink ref="A44" r:id="rId38" display="https://www.miljobs.ch/fr/functions/soldat-de-lechelon-de-conduite"/>
+    <hyperlink ref="A45" r:id="rId39" display="https://www.miljobs.ch/fr/functions/soldat-de-radar"/>
+    <hyperlink ref="A46" r:id="rId40" display="https://www.miljobs.ch/fr/functions/soldat-de-renseignement-des-forces-aeriennes"/>
+    <hyperlink ref="A47" r:id="rId41" display="https://www.miljobs.ch/fr/functions/soldat-de-telematique"/>
+    <hyperlink ref="A48" r:id="rId42" display="https://www.miljobs.ch/fr/functions/soldat-de-telematique-candidat-specialiste-de-langues"/>
+    <hyperlink ref="A49" r:id="rId43" display="https://www.miljobs.ch/fr/functions/soldat-dengins-guides-stinger"/>
+    <hyperlink ref="A50" r:id="rId44" display="https://www.miljobs.ch/fr/functions/soldat-dhopital-technique"/>
+    <hyperlink ref="A51" r:id="rId45" display="https://www.miljobs.ch/fr/functions/soldat-douvrage"/>
+    <hyperlink ref="A52" r:id="rId46" display="https://www.miljobs.ch/fr/functions/soldat-sanitaire-region-medico-militaire"/>
+    <hyperlink ref="A53" r:id="rId47" display="https://www.miljobs.ch/fr/functions/soldat-veterinaire"/>
+    <hyperlink ref="A54" r:id="rId48" display="https://www.miljobs.ch/fr/functions/automobiliste"/>
+    <hyperlink ref="A55" r:id="rId49" display="https://www.miljobs.ch/fr/functions/automobiliste-vehicules-speciaux"/>
+    <hyperlink ref="A56" r:id="rId50" display="https://www.miljobs.ch/fr/functions/conducteur-de-chiens"/>
+    <hyperlink ref="A57" r:id="rId51" display="https://www.miljobs.ch/fr/functions/soldat-de-la-circulation"/>
+    <hyperlink ref="A58" r:id="rId52" display="https://www.miljobs.ch/fr/functions/canonnier-lance-mines"/>
+    <hyperlink ref="A59" r:id="rId53" display="https://www.miljobs.ch/fr/functions/fantassin"/>
+    <hyperlink ref="A60" r:id="rId54" display="https://www.miljobs.ch/fr/functions/soldat-sanitaire"/>
+    <hyperlink ref="A61" r:id="rId55" display="https://www.miljobs.ch/fr/functions/soldat-dartillerie"/>
+    <hyperlink ref="A62" r:id="rId56" display="https://www.miljobs.ch/fr/functions/soldat-daviation-soldat-daerodrome"/>
+    <hyperlink ref="A63" r:id="rId57" display="https://www.miljobs.ch/fr/functions/conducteur-de-vehicules-a-chenilles-de-lartillerie"/>
+    <hyperlink ref="A64" r:id="rId58" display="https://www.miljobs.ch/fr/functions/fantassin-dequipage"/>
+    <hyperlink ref="A65" r:id="rId59" display="https://www.miljobs.ch/fr/functions/sanitaire-dunite"/>
+    <hyperlink ref="A66" r:id="rId60" display="https://www.miljobs.ch/fr/functions/sanitaire-dunite-conducteur-c1"/>
+    <hyperlink ref="A67" r:id="rId61" display="https://www.miljobs.ch/fr/functions/sapeur"/>
+    <hyperlink ref="A68" r:id="rId62" display="https://www.miljobs.ch/fr/functions/soldat-dequipage-de-chars"/>
+    <hyperlink ref="A69" r:id="rId63" display="https://www.miljobs.ch/fr/functions/soldat-de-chars"/>
+    <hyperlink ref="A70" r:id="rId64" display="https://www.miljobs.ch/fr/functions/soldat-de-chars-dappui"/>
+    <hyperlink ref="A71" r:id="rId65" display="https://www.miljobs.ch/fr/functions/soldat-de-sauvetage"/>
+    <hyperlink ref="A72" r:id="rId66" display="https://www.miljobs.ch/fr/functions/soldat-de-surete"/>
+    <hyperlink ref="A73" r:id="rId67" display="https://www.miljobs.ch/fr/functions/soldat-du-train"/>
+    <hyperlink ref="A74" r:id="rId68" display="https://www.miljobs.ch/fr/functions/soldat-de-la-police-militaire"/>
+    <hyperlink ref="A75" r:id="rId69" display="https://www.miljobs.ch/fr/functions/pilote-militaire-fonction-professionnelle"/>
+    <hyperlink ref="A76" r:id="rId70" display="https://www.miljobs.ch/fr/functions/eclaireur-parachutiste"/>
+    <hyperlink ref="A77" r:id="rId71" display="https://www.miljobs.ch/fr/functions/sapeur-de-chars"/>
+    <hyperlink ref="A78" r:id="rId72" display="https://www.miljobs.ch/fr/functions/soldat-sport"/>
+    <hyperlink ref="A79" r:id="rId73" display="https://www.miljobs.ch/fr/functions/explorateur"/>
+    <hyperlink ref="A80" r:id="rId74" display="https://www.miljobs.ch/fr/functions/eclaireur"/>
+    <hyperlink ref="A81" r:id="rId75" display="https://www.miljobs.ch/fr/functions/specialiste-de-montagne"/>
+    <hyperlink ref="A82" r:id="rId76" display="https://www.miljobs.ch/fr/functions/grenadier"/>
+    <hyperlink ref="A83" r:id="rId77" display="https://www.miljobs.ch/fr/functions/grenadier-de-chars"/>
+    <hyperlink ref="A84" r:id="rId78" display="https://www.miljobs.ch/fr/functions/grenadier-de-la-police-militaire"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId79"/>
 </worksheet>
 </file>
</xml_diff>